<commit_message>
- reformat csv output
</commit_message>
<xml_diff>
--- a/matching/src/planilhas/telefonia-smartphone-classificados-ewerton.xlsx
+++ b/matching/src/planilhas/telefonia-smartphone-classificados-ewerton.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5340" windowWidth="21630" windowHeight="5385"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="telefonia-smartphones-marcados-" sheetId="1" r:id="rId1"/>
@@ -28,25 +28,25 @@
     <t>Lg</t>
   </si>
   <si>
-    <t>LG OPTIMUS L1 II TRI</t>
+    <t>OPTIMUS L1 II TRI</t>
   </si>
   <si>
     <t>Smartphone LG G3 Beat Dual D724 Dual Chip Desbloqueado Android 4.4 Tela 5 8GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG G3 BEAT DUAL</t>
+    <t>G3 BEAT DUAL</t>
   </si>
   <si>
     <t>Smartphone LG Triple L20 D107 Android 4.4 Tela 3 4GB 3G Wi-Fi Camera 2MP - Preto e Grafite</t>
   </si>
   <si>
-    <t>LG TRIPLE L20</t>
+    <t>TRIPLE L20</t>
   </si>
   <si>
     <t>Smartphone LG G4 Desbloqueado Android 5.0 Tela 5.5 32GB 4G Wi-Fi Camera 16MP Hexa Core - Branco</t>
   </si>
   <si>
-    <t>LG G4</t>
+    <t>G4</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E3 Dual Chip Desbloqueado Android 4.4 Tela 4.5 4GB Camera de 5MP GPS - Branco</t>
@@ -55,7 +55,7 @@
     <t>Sony</t>
   </si>
   <si>
-    <t>SONY XPERIA E3</t>
+    <t>XPERIA E3</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 800 Desbloqueado Claro - Preto GSM Tela Curva 3.7 AMOLED Processador 1.4GHz 3G Wi-Fi Camera 8 MP com Dual-LED Flash e lente Carl Zeiss Memoria interna de 16GB e gratis 7GB de armazenamento no Sky Drive</t>
@@ -64,19 +64,19 @@
     <t>Nokia</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 800</t>
+    <t>LUMIA 800</t>
   </si>
   <si>
     <t>Smartphone Nokia C5-03 Desbloqueado Claro, Cinza / Prata, Tela 3.2, Camera 5.0MP, 3G, Wi-Fi, Memoria Interna 40MB e Cartao 2GB</t>
   </si>
   <si>
-    <t>NOKIA C5</t>
+    <t>C5</t>
   </si>
   <si>
     <t>Smartphone LG D340 L70 Tri Chip Android 4.4 KitKat Tela 4.5 4GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG L70</t>
+    <t>L70</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto X 2a Geracao Desbloqueado Android 4.4 Tela 5.2 32GB 4G Wi-Fi Camera 13MP GPS - Branco Bambu</t>
@@ -85,7 +85,7 @@
     <t>Motorola</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO X</t>
+    <t>MOTO X</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Gran 2 Duos Dual Chip Desbloqueado Android 4.3 Tela 5.3 Camera 8MP TV Digital - Preto</t>
@@ -94,37 +94,37 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN 2 DUOS</t>
+    <t>GALAXY GRAN 2 DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Core Plus Dual Chip Desbloqueado Android 4.3 Tela 4.3 Preto 3G Wi-Fi Camera 5MPx TV Digital - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY CORE PLUS</t>
+    <t>GALAXY CORE PLUS</t>
   </si>
   <si>
     <t>Smartphone Motorola RAZR i Android 4.0 Tela 4.3 8GB 3G Wi-Fi Camera de 8MP GPS - Branco</t>
   </si>
   <si>
-    <t>MOTOROLA RAZR I</t>
+    <t>RAZR I</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L3 Preto - GSM, Android 2.3, Processador 600 Mhz, 3G, Wi-Fi, Camera 3.2MP, Filmadora, Bluetooth 2.1, MP3 Player e Radio FM</t>
   </si>
   <si>
-    <t>LG OPTIMUS L3</t>
+    <t>OPTIMUS L3</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L5 E612 Preto Desbloqueado Claro - Android 4.0, Super bateria, Touchscreen 4, Camera 5.0MP, 3G, Wi-Fi e Memoria interna de 4GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS L5</t>
+    <t>OPTIMUS L5</t>
   </si>
   <si>
     <t>Smartphone LG G Flex Desbloqueado Android 4.2 Tela 6 32GB 4G Wi-Fi Camera 13MP - Preto</t>
   </si>
   <si>
-    <t>LG G FLEX</t>
+    <t>G FLEX</t>
   </si>
   <si>
     <t>Smartphone Asus ZenFone 6 Dual Chip Desbloqueado Android 4.4 Tela 6 16GB 3G Wi-Fi Camera 13MP - Preto</t>
@@ -133,31 +133,31 @@
     <t>Asus</t>
   </si>
   <si>
-    <t>ASUS ZENFONE 6</t>
+    <t>ZENFONE 6</t>
   </si>
   <si>
     <t>Smartphone LG Optimus me P350 Desbloqueado Claro Android 2.2 3G WiFi Touch GPS Cam 3MP 2GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS ME</t>
+    <t>OPTIMUS ME</t>
   </si>
   <si>
     <t>Smartphone LG C570 Cinza - GSM c/ Tecnologia 3G, Wi-Fi, Teclado QWERTY, GPS, Camera 2MP c/ Zoom 3x, Filmadora, MP3 Player, Radio FM, Bluetooth, Fone, Cabo de Dados e Cartao 2GB</t>
   </si>
   <si>
-    <t>LG CINZA</t>
+    <t>CINZA</t>
   </si>
   <si>
     <t>Smartphone Dual Chip LG Optimus L5 Dual Preto Android 4.0 Desbloqueado Tim - Camera 5.0MP 3G Wi-Fi Memoria Interna 4GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS L5 DUAL</t>
+    <t>OPTIMUS L5 DUAL</t>
   </si>
   <si>
     <t>Smartphone LG L9 Desbloqueado Tim Preto - Android 4.0 - Processador Dual Core 1GHz, Tela 4.7, Camera 5.0MP, 3G, Wi-Fi, Memoria Interna 4GB e Cartao 4GB</t>
   </si>
   <si>
-    <t>LG L9</t>
+    <t>L9</t>
   </si>
   <si>
     <t>Smartphone LG L9 Desbloqueado Tim Branco - Android 4.0 - Processador Dual Core 1GHz, Tela 4.7, Camera 5.0MP, 3G, Wi-Fi, Memoria Interna 4GB e Cartao 4GB</t>
@@ -166,25 +166,25 @@
     <t>Smartphone Samsung Galaxy Gran Prime Duos Chip Desbloqueado Android 4.4 Kit Kat Tela 5 8GB 3G Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN PRIME DUOS CHIP</t>
+    <t>GALAXY GRAN PRIME DUOS CHIP</t>
   </si>
   <si>
     <t>Smartphone Motorola Novo Moto X Desbloqueado Android 4.4 Tela 5.2 32GB 4G Wi-Fi Camera 13MP GPS - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA NOVO MOTO X</t>
+    <t>NOVO MOTO X</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z1 Desbloqueado Preto Android 4.2 4G Camera 20MP 16GB</t>
   </si>
   <si>
-    <t>SONY XPERIA Z1</t>
+    <t>XPERIA Z1</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L3 Dual E405 Desbloqueado Oi  Rosa GSM  Dual Chip  Android 2.3 Processador  600 Mhz  3G  Wi-Fi Camera 3.2MP Filmadora Bluetooth 2.1 MP3 Player e Radio FM</t>
   </si>
   <si>
-    <t>LG OPTIMUS L3 DUAL</t>
+    <t>OPTIMUS L3 DUAL</t>
   </si>
   <si>
     <t>Smartphone Blu Studio 5.0 D530 Anatel/Generic Dual Sim 3G Preto</t>
@@ -193,25 +193,25 @@
     <t>Blu</t>
   </si>
   <si>
-    <t>BLU STUDIO 5.0 ANATEL GENERIC</t>
+    <t>STUDIO 5.0 ANATEL GENERIC</t>
   </si>
   <si>
     <t>Smartphone Nokia E63 Azul - GSM c/ Tecnologia 3G, Wi-Fi, Teclado Qwerty, Camera 2.0MP c/ zoom e Flash LED, Filmadora, MP3 Player, Radio FM, Bluetooth Estereo 2.0, Viva-Voz e Fone</t>
   </si>
   <si>
-    <t>NOKIA E63</t>
+    <t>E63</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 520 Desbloqueado Windows Phone 8 Tela 4 8GB 3G Wi-Fi Camera 5MP GPS - Branco</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 520</t>
+    <t>LUMIA 520</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L7 II Dual Chip Desbloqueado Android 4.1 Tela 4.3 4GB 3G Wi-Fi Camera 8MP - Branco + Cartao de Memoria 4GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS L7 II</t>
+    <t>OPTIMUS L7 II</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L3 E405 Desbloqueado Tim, Branco, Dual Chip - Android 2.3, Processador 600 Mhz, Tela 3.2, Camera 3.2MP, 3G, Wi-Fi e Memoria Interna 2GB</t>
@@ -220,19 +220,19 @@
     <t>Smartphone Sony Xperia E1 Desbloqueado Vivo Android 4.3 Tela 4 4GB 3G Wi-Fi Camera 3MP - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA E1</t>
+    <t>XPERIA E1</t>
   </si>
   <si>
     <t>Smartphone LG L40 D180 TV Tri Chip Desbloqueado Android 4.4 Tela 3.5 4GB 3G Wi-Fi Camera 3MP TV Digital - Branco</t>
   </si>
   <si>
-    <t>LG L40 TV</t>
+    <t>L40 TV</t>
   </si>
   <si>
     <t>Smartphone Motorola Motosmart Me XT303. Desbloqueado. GSM. Preto - Android 2.3. Touchscreen 3.2". Camera de 2MP. 3G. Wi Fi. Bluetooth. GPS. MP3 Player. Radio FM. Cartao de Memoria de 4GB</t>
   </si>
   <si>
-    <t>MOTOROLA MOTOSMART ME</t>
+    <t>MOTOSMART ME</t>
   </si>
   <si>
     <t>Smartphone LG E400f Optimus L3 Desbloqueado Tim Preto - GSM Android 2.3, Processador 600 Mhz 3G Wi-Fi Camera 3.2MP Filmadora Bluetooth 2.1 MP3 Player Radio FM Memoria interna de 2 GB</t>
@@ -241,61 +241,61 @@
     <t>Smartphone LG P500 Desbloqueado Claro Preto - GSM com Sistema Operacional Android 2.2, Tecnologia 3G, Wi-Fi, GPS, TouchScreen c/ Tela de 3.2", Camera 3.2MP, Filmadora, MP3 Player, Radio FM, Bluetooth, Fone, Cabo de Dados e Cartao de 2GB</t>
   </si>
   <si>
-    <t>LG P500</t>
+    <t>P500</t>
   </si>
   <si>
     <t>Smartphone Nokia E5. Desbloqueado Vivo. Prata. Tela 2.36". Camera 5MP. 3G. Wi Fi. Memoria Interna 250MB e Cartao 2GB</t>
   </si>
   <si>
-    <t>NOKIA E5</t>
+    <t>E5</t>
   </si>
   <si>
     <t>Smartphone Lg Leon Tv H326tv Tela De 4-5 8gb Dual Chip Quad Core Android 5-0 C-Mera 8mp Tit-Nio</t>
   </si>
   <si>
-    <t>LG LEON TV TELA DE 4-5</t>
+    <t>LEON TV TELA DE 4-5</t>
   </si>
   <si>
     <t>Smartphone LG L80 Dual Chip Desbloqueado Tim Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP TV Digital Preto</t>
   </si>
   <si>
-    <t>LG L80</t>
+    <t>L80</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 4G I9515 16GB Desbloqueado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S4</t>
+    <t>GALAXY S4</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Mini Duos Dual Chip Desbloqueado Tim Android 4.4 Tela 4.5" 16GB 3G Wi-Fi Camera 8MP GPS - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5 MINI DUOS</t>
+    <t>GALAXY S5 MINI DUOS</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L1 II E410 Desbloqueado Claro Android 4.1 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Branco</t>
   </si>
   <si>
-    <t>LG OPTIMUS L1 II</t>
+    <t>OPTIMUS L1 II</t>
   </si>
   <si>
     <t>Smartphone LG Pro Lite, Desbloqueado, Branco, Android 4,1,3G, Wi-Fi, Camera 8 MP, Memoria Interna 8GB, GPS</t>
   </si>
   <si>
-    <t>LG PRO LITE</t>
+    <t>PRO LITE</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia ZQ Desbloqueado Oi Preto - Android 4.1 4G Wi-Fi Camera 13MP Memoria Interna 16GB GPS NFC</t>
   </si>
   <si>
-    <t>SONY XPERIA ZQ</t>
+    <t>XPERIA ZQ</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S II Desbloqueado Vivo - Android 2.3 Dual Core Cam 8MP 3G  Wi Fi 16GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S II</t>
+    <t>GALAXY S II</t>
   </si>
   <si>
     <t>Smartphone LG L9 Desbloqueado Tim Preto - Android 4.0 - Tela 4.7" Camera 5.0MP 3G Wi-Fi</t>
@@ -304,13 +304,13 @@
     <t>Smartphone Sony Xperia SP Desbloqueado Claro Branco Android 4.1 4G Camera 8MP Memoria Interna 8GB GPS NFC</t>
   </si>
   <si>
-    <t>SONY XPERIA SP</t>
+    <t>XPERIA SP</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 Zoom Branco Android 4.2 3G Desbloqueado - Camera 16MP Camera Wi-Fi GPS Memoria 8GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S4 ZOOM</t>
+    <t>GALAXY S4 ZOOM</t>
   </si>
   <si>
     <t>Smartphone LG E400f Optimus L3  Desbloqueado Tim Branco - GSM  Android 2.3, Processador 600 Mhz  3G Wi-Fi  Camera 3.2MP Filmadora Bluetooth 2.1 MP3 Player Radio FM Memoria interna de 2 GB</t>
@@ -322,7 +322,7 @@
     <t>Smartphone LG P880 Optimus Preto 3G Desbloqueado Camera 8MP Wi-Fi Memoria Interna de 16 GB Expansivel ate 32 GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS</t>
+    <t>OPTIMUS</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L5 Dual Desbloqueado Rosa. Dual Chip. Android 4.0. Tela 4". Camera 5.0MP. 3G. Wi Fi. Memoria Interna 4GB</t>
@@ -334,7 +334,7 @@
     <t>Smartphone Motorola Spice Desbloqueado Oi Preto - Android 2.1, Tela 3", Camera 3.2MP, 3G, Wi-Fi e Cartao 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA SPICE</t>
+    <t>SPICE</t>
   </si>
   <si>
     <t>Smartphone Nokia E5 Desbloqueado, Branco - Symbian - Tela 2.3", Camera 5MP, 3G, Wi-Fi, Memoria Interna 250MB e Cartao 2GB</t>
@@ -343,25 +343,25 @@
     <t>Smartphone LG P970 Optimus Black Desbloqueado Claro, Preto - Android 2.2, Processador 1GHZ, Tela 4", Camera de 5MP, 3G, Wi-Fi e Memoria Interna 1GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS BLACK</t>
+    <t>OPTIMUS BLACK</t>
   </si>
   <si>
     <t>Smartphone LG Optimus Pro C660, Desbloqueado TIM -  Android 2.3, Tecnologia 3G, Wi-Fi, Camera 3.2 MP TouchScreen, Teclado Qwerty, GPS, Filmadora, MP3 Player, Radio FM, Bluetooth, Fone, Cabo de Dados e Cartao de Memoria 2GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS PRO</t>
+    <t>OPTIMUS PRO</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Desbloqueado Android 4.4.2 Tela 5.1" 16GB 4G Wi-Fi Camera 16 MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5</t>
+    <t>GALAXY S5</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Duos SM-G900M Dual Chip Desbloqueado Android 4.4 16GB 4G Wi-Fi GPS - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5 DUOS SM</t>
+    <t>GALAXY S5 DUOS SM</t>
   </si>
   <si>
     <t>Smartphone LG L70 D325 Dual Chip Desbloqueado Android 4.4 Tela 4.5" 4GB 3G Wi-Fi Camera 8MP - Preto</t>
@@ -370,7 +370,7 @@
     <t>Smartphone Samsung Galaxy S III Mini Desbloqueado Android 4.2 Tela 4" 8GB 3G Wi-Fi Camera 5 MP - Grafite</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S III MINI</t>
+    <t>GALAXY S III MINI</t>
   </si>
   <si>
     <t>Smartphone LG L40 D180 TV Tri Chip Desbloqueado Android 4.4 Tela 3.5" 4GB 3G Wi-Fi Camera 3MP TV Digital - Preto</t>
@@ -382,37 +382,37 @@
     <t>Smartphone Samsung Galaxy A3 Duos Dual Chip Desbloqueado Android 4.4 Tela 4.5" 16GB 4G Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A3 DUOS</t>
+    <t>GALAXY A3 DUOS</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 630 Windows 8.1 Tela 4.5" 8GB 3G Wi Fi Camera 5MP GPS TV Digital - Preto</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 630</t>
+    <t>LUMIA 630</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Note 4, 4g 32gb, Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY NOTE 4</t>
+    <t>GALAXY NOTE 4</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z3 Compact Desbloqueado Android 4.4 Kit Kat Tela 4.6" 16GB 4G Wi-Fi Camera 20.7MP - Laranja</t>
   </si>
   <si>
-    <t>SONY XPERIA Z3 COMPACT</t>
+    <t>XPERIA Z3 COMPACT</t>
   </si>
   <si>
     <t>Smartphone LG Prime Plus TV Dual Chip Desbloqueado Android 5.0 Tela 5" 8GB 3G Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG PRIME PLUS TV</t>
+    <t>PRIME PLUS TV</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy E5 Duos Dual Chip Desbloqueado Android 4.4 Tela Amoled HD 5" 16GB 4G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY E5 DUOS</t>
+    <t>GALAXY E5 DUOS</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia ZQ Desbloqueado Vivo Preto - Android 4.1 4G Wi-Fi Camera 13MP Memoria Interna 16GB GPS NFC</t>
@@ -421,61 +421,61 @@
     <t>Smartphone Motorola Novo Moto G Dual Chip XT 1068 Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera de 8MP - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA NOVO MOTO G</t>
+    <t>NOVO MOTO G</t>
   </si>
   <si>
     <t>Smartphone Lg Volt Tv H422tv Titanio, Android 5.0 Lollipop, Tela 4.7, Camera 8mp, Mem 8gb - 3g</t>
   </si>
   <si>
-    <t>LG VOLT TV</t>
+    <t>VOLT TV</t>
   </si>
   <si>
     <t>Smartphone Lg Volt Tv Dual H422 Desbloqueado Azul</t>
   </si>
   <si>
-    <t>LG VOLT TV DUAL</t>
+    <t>VOLT TV DUAL</t>
   </si>
   <si>
     <t>Smartphone LG Optimus HUB E510 - Android 2.3. Cam 5.0MP. Wi Fi. Bluetooth 3.0. 3G e Cartao de Memoria 4GB - Desbloqueado Tim</t>
   </si>
   <si>
-    <t>LG OPTIMUS HUB</t>
+    <t>OPTIMUS HUB</t>
   </si>
   <si>
     <t>Smartphone Motorola Novo Moto G DTV Colors Dual Chip XT 1069 Desbloqueado Android 4.4 Tela 5" 16GB 3G Wi-Fi Camera de 8MP - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA NOVO MOTO G DTV COLORS</t>
+    <t>NOVO MOTO G DTV COLORS</t>
   </si>
   <si>
     <t>Smartphone LG D410 L90 Dual Chip Desbloqueado Android 4.4 Kit Kat Tela 4.7" 8GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG L90</t>
+    <t>L90</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 Mini Desbloqueado Vivo Android 4.2 Tela 4" 8GB 4G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S4 MINI</t>
+    <t>GALAXY S4 MINI</t>
   </si>
   <si>
     <t>Smartphone Sony Ericsson Xperia Arc S, Desbloqueado Tim, Prata - Android 2.3, Processador 1.4GHz, Tela 4.2", Camera 8.0MP, 3G, Wi-Fi, Memoria Interna 320MB e Cartao 16 GB</t>
   </si>
   <si>
-    <t>SONY XPERIA ARC S</t>
+    <t>XPERIA ARC S</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Play Desbloqueado Tim Android 2.3 Tela 4" 400MB 3G Wi-Fi Camera 5.1MP - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA PLAY</t>
+    <t>XPERIA PLAY</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia S Desbloqueado Android 4.0 Tela 4.3" 32GB 3G Wi-Fi Camera 12MP GPS - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA S</t>
+    <t>XPERIA S</t>
   </si>
   <si>
     <t>Smartphone Nokia C5-03 Desbloqueado Claro Tela 3.2" 40MB 3G Wi-Fi Camera 5MP Branco e Lilas + Cartao 2GB</t>
@@ -484,13 +484,13 @@
     <t>Smartphone Samsung Galaxy Fame Lite S6790 Desbloqueado Vivo Android 4.1 Tela 3.5" 4GB 3G Wi-Fi Camera 3MP GPS - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY FAME LITE</t>
+    <t>GALAXY FAME LITE</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia M Dual Desbloqueado Tim Android 4.1 Tela 4" 4GB 3G Wi-Fi Camera 5MP GPS - Branco</t>
   </si>
   <si>
-    <t>SONY XPERIA M DUAL</t>
+    <t>XPERIA M DUAL</t>
   </si>
   <si>
     <t>Smartphone Motorola MOTOSMART ME XT305, Desbloqueado, Branco, Dual Chip - Android 2.3, Display 3.2", Touchscreen, Camera de 2MP, Filmadora, 3G, Wi-Fi, Bluetooth, MP3 Player, Radio FM, GPS, Memoria interna de 512MB, Cartao de Memoria 4GB</t>
@@ -499,13 +499,13 @@
     <t>Smartphone LG G3 Stylus D690 Dual Chip Desbloqueado Android 4.4 Tela 5.5" 8GB 3G Wi-Fi Camera 13MP - Branco</t>
   </si>
   <si>
-    <t>LG G3 STYLUS</t>
+    <t>G3 STYLUS</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto G com 4G Desbloqueado Android 4.4 Tela 4.5" 8GB 4G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO G COM</t>
+    <t>MOTO G COM</t>
   </si>
   <si>
     <t>Smartphone Sony Ericsson X1 XPERIA Desbloqueado Preto Wi Fi 3G Camera 3.2 MP</t>
@@ -514,7 +514,7 @@
     <t>Sony Ericsson</t>
   </si>
   <si>
-    <t>SONY ERICSSON X1 XPERIA</t>
+    <t>X1 XPERIA</t>
   </si>
   <si>
     <t>Smartphone Apple iPhone 4S - Preto - GSM, Tela Touch 3.5" Full HD, iOS 5.0, Processador 1GHz Dual Core, 3G, Wi-Fi, SIRI, iCloud, GPS, Camera 8MP, Memoria interna de 32GB - Desbloqueado Tim</t>
@@ -523,13 +523,13 @@
     <t>Apple</t>
   </si>
   <si>
-    <t>APPLE IPHONE 4 S</t>
+    <t>IPHONE 4 S</t>
   </si>
   <si>
     <t>Smartphone LG L80 TV Single D375 Preto com Tela de 5 pol. TV Digital, Android 4.4</t>
   </si>
   <si>
-    <t>LG L80 TV SINGLE</t>
+    <t>L80 TV SINGLE</t>
   </si>
   <si>
     <t>Smartphone Alcatel Ot 5020 Roxo Dual Chip 3g Camera 5mp</t>
@@ -538,13 +538,13 @@
     <t>Alcatel</t>
   </si>
   <si>
-    <t>ALCATEL OT</t>
+    <t>OT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Young 2 Duos Tv G130bt Desbloqueado Cinza</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY YOUNG 2 DUOS TV</t>
+    <t>GALAXY YOUNG 2 DUOS TV</t>
   </si>
   <si>
     <t>Smartphone LG Optimus Desbloqueado TIM Preto - Android 4.0, Processador 800Mhz, Touchscreen 4", Camera 5.0 MP com Flash LED, Filmadora, 3G, Wi-Fi, MP3 Player, Radio FM, Bluetooth, GPS, Fone de Ouvido, Cabo de Dados, Memoria interna de 4GB</t>
@@ -553,13 +553,13 @@
     <t>Smartphone LG Optimus G Branco Android 4.1 3G Desbloqueado TIM Camera 13MP Wi-Fi Memoria Interna 32GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS G</t>
+    <t>OPTIMUS G</t>
   </si>
   <si>
     <t>Smartphone Lg Optimus F3 P655 4g Desbloqueado Vivo Preto</t>
   </si>
   <si>
-    <t>LG OPTIMUS F3</t>
+    <t>OPTIMUS F3</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L3 E405 Desbloqueado Tim, Preto, Dual Chip - Android 2.3, Processador 600 Mhz, Tela 3.2", Camera 3.2MP, 3G, Wi-Fi e Memoria Interna 2GB</t>
@@ -574,31 +574,31 @@
     <t>Smartphone Nokia Lumia 820 Desbloqueado Tim Branco Windows Phone 8 4G/Wi Fi Camera 8MP 8GB</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 820</t>
+    <t>LUMIA 820</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S III I9300 Grafite Blue Android 4.0 3G Desbloqueado Vivo - Camera 8MP Wi-Fi GPS Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S III</t>
+    <t>GALAXY S III</t>
   </si>
   <si>
     <t>Smartphone Blu Amour D290I Qband Dual Sim 3G 850/2100 Branco</t>
   </si>
   <si>
-    <t>BLU AMOUR QBAND</t>
+    <t>AMOUR QBAND</t>
   </si>
   <si>
     <t>Smartphone Blu Life Play L100I Qband Dual Sim 3G 850/2100 Cinza</t>
   </si>
   <si>
-    <t>BLU LIFE PLAY QBAND</t>
+    <t>LIFE PLAY QBAND</t>
   </si>
   <si>
     <t>Smartphone Blu Studio 5.0 C Hd, Android 4.4, Dual Chip, Camera 8mp, Mem 4gb, Tela 5.0, 3g - Amarel</t>
   </si>
   <si>
-    <t>BLU STUDIO 5.0 C HD</t>
+    <t>STUDIO 5.0 C HD</t>
   </si>
   <si>
     <t>Smartphone Blu Studio 5.0 C Hd, Android 4.4, Dual Chip, Camera 8mp, Mem 4gb, Tela 5.0, 3g - Azul</t>
@@ -613,67 +613,67 @@
     <t>Smartphone Samsung Galaxy S5 Debloqueado Branco 4G Android 4.4 Tela 5.1"</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5 DEBLOQUEADO</t>
+    <t>GALAXY S5 DEBLOQUEADO</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S6 G920i Desbloqueado Dourado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S6</t>
+    <t>GALAXY S6</t>
   </si>
   <si>
     <t>Smartphone Desbloqueado Samsung Galaxy Ace 4 Plus Duos Cinza</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE 4 PLUS DUOS CINZA</t>
+    <t>GALAXY ACE 4 PLUS DUOS CINZA</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A3 4g Duos, Sm-A300m/Ds, Quad Core 1.2 Ghz, Camera 8 Mp, Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A3</t>
+    <t>GALAXY A3</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy E7 Sm-E700 16 Gb 4g Duos Quad Core 1.2ghz Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY E7 SM</t>
+    <t>GALAXY E7 SM</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Fame Duos S6812 Grafite, Dual Chip, Android 4.1, Wi-Fi, 3g, Camera 5.0, T</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY FAME DUOS</t>
+    <t>GALAXY FAME DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Sm G900 M Azul, 16gb, Quad-Core 2.5ghz, Tela Full Hd 5.1 Polegadas, Ca</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5 SM M</t>
+    <t>GALAXY S5 SM M</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Trend Lite Gt-S7390 Desbloqueado Tela 4 3g Android 4.4 Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY TREND LITE GT</t>
+    <t>GALAXY TREND LITE GT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Win 2 Duos G360 Tv Desbloqueado Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY WIN 2 DUOS TV</t>
+    <t>GALAXY WIN 2 DUOS TV</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Siii I9300 Branco, 16gb, Camera 8mp  1.9mp Frontal, Tela 4.8 Polegadas,</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY SIII</t>
+    <t>GALAXY SIII</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A5 4g Duos, Sm-A500m/Ds, Quad Core 1.2 Ghz, Camera 13 Mp, Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A5</t>
+    <t>GALAXY A5</t>
   </si>
   <si>
     <t>Smartphone Microsoft Lumia 435 Dual Desbloqueado Branco</t>
@@ -682,13 +682,13 @@
     <t>Microsoft</t>
   </si>
   <si>
-    <t>MICROSOFT LUMIA 435 DUAL</t>
+    <t>LUMIA 435 DUAL</t>
   </si>
   <si>
     <t>Smartphone LG Leon Dual Chip Desbloqueado Android 5.0 Lollipop Tela 4.5" 8GB 3G Camera 5MP TV Digital - Branco</t>
   </si>
   <si>
-    <t>LG LEON</t>
+    <t>LEON</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z3 Compact Preto</t>
@@ -703,13 +703,13 @@
     <t>Blackberry</t>
   </si>
   <si>
-    <t>BLACKBERRY Z10</t>
+    <t>Z10</t>
   </si>
   <si>
     <t>Smartphone LG Volt Dual H422 Dual Chip Desbloqueado Android 5.0 Lollipop Tela 4.7" 8GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG VOLT DUAL</t>
+    <t>VOLT DUAL</t>
   </si>
   <si>
     <t>Smartphone LG G3 Beat Dual D724 Dual Chip Android 4.4 Desbloqueado Android 4.4 Tela 5" 3G Wi-Fi Camera 8MP GPS - Titanio</t>
@@ -718,7 +718,7 @@
     <t>Smartphone Alcatel Pop C1 Dualchip 4015N Desbloqueado Android 4.2 Tela 3.5" 4GB Micro SD ate 32GB Camera de 2MP GPS - Azul</t>
   </si>
   <si>
-    <t>ALCATEL POP C1 DUALCHIP N</t>
+    <t>POP C1 DUALCHIP N</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z3 Compact Desbloqueado Android 4.4 Tela 4.6" 16GB 4G Wi-Fi Camera 20.7MP - Preto</t>
@@ -727,7 +727,7 @@
     <t>Smartphone Lg Optimus L5 Ii E450 Branco, 4 Polegadas, Android 4.1, Processador 1ghz, Camera De 5mp,</t>
   </si>
   <si>
-    <t>LG OPTIMUS L5 II</t>
+    <t>OPTIMUS L5 II</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Note 4 Desbloqueado Android 4.4 Tela 5.7" 32GB Wi-Fi Camera de 16MP - Preto</t>
@@ -739,7 +739,7 @@
     <t>Smartphone LG L50 Dual Chip Desbloqueado Tim Android 4.4 Tela 4" 4GB Wi-Fi 3G Camera 5MP com TV Digital - Preto e Azul</t>
   </si>
   <si>
-    <t>LG L50</t>
+    <t>L50</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto X Desbloqueado Android 4.2.2 Tela 4.7" 16GB Camera 10MP e Frontal 2MP - Bambu</t>
@@ -760,31 +760,31 @@
     <t>Smartphone Lg Leon Tv H326 Desbloqueado Azul/Preto</t>
   </si>
   <si>
-    <t>LG LEON TV</t>
+    <t>LEON TV</t>
   </si>
   <si>
     <t>Smartphone Motorola XT687 AtrixTV, Desbloqueado, Cinza, Dual Chip - Android 4.0, Processador 1GHz, Tela 4", Camera 8.0MP, 3G, Wi-Fi  e Cartao 4GB</t>
   </si>
   <si>
-    <t>MOTOROLA ATRIXTV</t>
+    <t>ATRIXTV</t>
   </si>
   <si>
     <t>Smartphone Motorola XT321 Defy Mini, Rosa, GSM, Dual Chip - Android 2.3, Camera 3MP com Flash, Filmadora, Camera Frontal VGA, 3G, Wi-Fi, Bluetooth, Touch 3.2", Cartao de Memoria de 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA DEFY MINI</t>
+    <t>DEFY MINI</t>
   </si>
   <si>
     <t>Smartphone Dual Chip Motorola Razr D1 Desbloqueado Branco TV Android 4.1 Camera 5MP 3G Wi-Fi</t>
   </si>
   <si>
-    <t>MOTOROLA RAZR D1</t>
+    <t>RAZR D1</t>
   </si>
   <si>
     <t>Smartphone Motorola Razr D3 Dual Chip Branco 3G Android 4.1 Camera 8MP Wi-Fi</t>
   </si>
   <si>
-    <t>MOTOROLA RAZR D3</t>
+    <t>RAZR D3</t>
   </si>
   <si>
     <t>Smartphone Motorola Razr D3 Dual Chip Android 4.1 Tela 4" 3G Wi-Fi Camera 8MP - Preto</t>
@@ -793,7 +793,7 @@
     <t>Smartphone Moto G Music Edition Dual Chip Desbloqueado Android 4.3 Tela 4.5" 16GB 3G Wi-Fi Camera 5MP + Fone de Ouvido Bluetooth Tracks Air Sol Republic - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO G MUSIC EDITION</t>
+    <t>MOTO G MUSIC EDITION</t>
   </si>
   <si>
     <t>Smartphone Motorola Razr D3 Branco Android 4.1 3G - Camera 8MP Wi-Fi GPS 4GB</t>
@@ -805,7 +805,7 @@
     <t>Smartphone Motorola Moto G Desbloqueado TIM Android 4.3 Tela 4.5" 8GB 3G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO G</t>
+    <t>MOTO G</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto G Dual Chip Desbloqueado Tim Android 4.3 Tela 4.5" 8GB 3G Wi-Fi Camera 5MP GPS - Preto</t>
@@ -817,19 +817,19 @@
     <t>Smartphone LG Monster High E400f OpTimus L3 Android 2.3 Tela 3.2" 2GB 3G Wi-Fi Camera 3.2MP - Preto</t>
   </si>
   <si>
-    <t>LG MONSTER HIGH OPTIMUS L3</t>
+    <t>MONSTER HIGH OPTIMUS L3</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus F5 Desbloqueado Claro Tela 4.3" 8GB Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>LG OPTIMUS F5</t>
+    <t>OPTIMUS F5</t>
   </si>
   <si>
     <t>Smartphone LG G2 Desbloqueado Android 4.2 Tela 5.2" 16GB 4G Wi-Fi Camera 13MP - Preto</t>
   </si>
   <si>
-    <t>LG G2</t>
+    <t>G2</t>
   </si>
   <si>
     <t>Smartphone Motorola RAZR i, Desbloqueado TIM Preto, Processador Intel Inside 2GHz, Tela AMOLED Advanced 4.3", Touchscreen, Android 4.0, Camera de 8MP , Camera Frontal VGA, Gravacao Full HD, 3G, Wi-Fi, Bluetooth, GPS, NFC, Memoria Interna de 8GB</t>
@@ -838,7 +838,7 @@
     <t>Smartphone Motorola Defy Pro XT560, GSM, Prata, QWERTY, Android 2.3, Camera 5.0MP, 3G, Wi-Fi, Bluetooth, Cartao de memoria 2GB, Desbloqueado TIM</t>
   </si>
   <si>
-    <t>MOTOROLA DEFY PRO</t>
+    <t>DEFY PRO</t>
   </si>
   <si>
     <t>Smartphone Dual Chip Motorola RAZR D3 Branco Android 4.1 Desbloqueado TIM - Camera 8MP Wi-Fi 3G Processador Dual Core 1,2 Ghz e Memoria Interna 4GB</t>
@@ -850,7 +850,7 @@
     <t>Smartphone LG Optimus E465 L4 II Desbloqueado Claro Preto</t>
   </si>
   <si>
-    <t>LG OPTIMUS L4 II</t>
+    <t>OPTIMUS L4 II</t>
   </si>
   <si>
     <t>Smartphone LG E405f Optimus L3 Dual Chip Desbloqueado Oi - Branco - GSM  Android 2.3  Processador 600 Mhz 3G Wi-Fi  Camera 3.2MP Filmadora  Bluetooth 2.1  MP3 Player Radio FM Memoria interna de 2 GB</t>
@@ -859,13 +859,13 @@
     <t>Smartphone Motorola MB525 Defy Desbloqueado Claro, Preto - Android 2.1, Tela 3.7", Camera 5.0MP, 3G, Wi-Fi, Memoria Interna 2GB e Cartao 8GB</t>
   </si>
   <si>
-    <t>MOTOROLA DEFY</t>
+    <t>DEFY</t>
   </si>
   <si>
     <t>Smartphone Motorola Fire. Branco. Dual Chip.  Touchscreen 2.8". Android 2.3. Cam 3MP. 3G. Wi Fi. GPS + Cartao Memoria 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA FIRE</t>
+    <t>FIRE</t>
   </si>
   <si>
     <t>Smartphone Motorola MOTOSMART ME XT305, Desbloqueado Tim, Branco, Dual Chip - Android 2.3, Display 3.2", Touchscreen, Camera de 2MP, Filmadora, 3G, Wi-Fi, Bluetooth, MP3 Player, Radio FM, GPS, Memoria interna de 512MB, Cartao de Memoria 4GB</t>
@@ -886,7 +886,7 @@
     <t>Smartphone LG Optimus L3 II Preto  - Android 4.1 3G Desbloqueado Camera 3MP Wi-Fi GPS</t>
   </si>
   <si>
-    <t>LG OPTIMUS L3 II</t>
+    <t>OPTIMUS L3 II</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L1 II Tri E475 Tri Chip Desbloqueado Android 4.1 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Branco</t>
@@ -904,7 +904,7 @@
     <t>Smartphone LG Nexus 5 Android 4.4 Tela 5" 16GB 4G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG NEXUS 5</t>
+    <t>NEXUS 5</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L3 II Branco - Android 4.1 3G Desbloqueado Claro - Camera 3MP Wi-Fi GPS</t>
@@ -922,13 +922,13 @@
     <t>Smartphone Motorola XT 300 Spice Desbloqueado Claro, Branco / Rosa - Android 2.1, Touch 3", Camera 3.2MP, 3G, Wi-Fi, Memoria Interna 512MB e Cartao 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA XT 300 SPICE</t>
+    <t>XT 300 SPICE</t>
   </si>
   <si>
     <t>Smartphone Motorola A953 Milestone 2 Desbloqueado TIM, Azul Marinho - Android 2.2, Touch 3.7, Camera 5.0MP c/ Flash LED Duplo, Filmadora HD, 3G, Wi-Fi, GPS, Bluetooth, MP3 Player, Bluetooth 2.1,Fone, Cabo de Dados, Cartao 8GB + Dock Station</t>
   </si>
   <si>
-    <t>MOTOROLA MILESTONE 2</t>
+    <t>MILESTONE 2</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L5 E612 Desbloqueado Oi Preto - 3G Wi Fi Android 4.0 Tela 4" Camera 5MP</t>
@@ -946,7 +946,7 @@
     <t>Smartphone Motorola RAZR HD Preto Android 4.0 4G - Camera 8MP, Camera Frontal 1.3MP, Wi-Fi, GPS, Processador Dual core 1.5 Ghz, Tela AMOLED HD 4.7", Bluetooth, Memoria interna de 16GB, Cartao de memoria de 16GB</t>
   </si>
   <si>
-    <t>MOTOROLA RAZR HD</t>
+    <t>RAZR HD</t>
   </si>
   <si>
     <t>Smartphone LG Optimus P350 Desbloqueado TIM, Prata - Android 2.2, Tela 2.8", 3G, WiFi, GPS, Camera 3.0MP, Memoria Interna 150MB e Cartao 2GB</t>
@@ -958,25 +958,25 @@
     <t>Smartphone Motorola DEFY Desbloq. TIM + Android 2.3 1GHz Wi Fi 3G GPS Cam 5MP 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA DEFY DESBLOQ</t>
+    <t>DEFY DESBLOQ</t>
   </si>
   <si>
     <t>Smartphone Motorola XT390 Motosmart Dual Chip - Cinza - GSM, Tela Touch 3.5", Android 2.3, 3G, Wi-Fi, Camera 3MP, Filmadora, MP3 Player, Radio FM, Incluso Cartao de Memoria de 4GB</t>
   </si>
   <si>
-    <t>MOTOROLA MOTOSMART</t>
+    <t>MOTOSMART</t>
   </si>
   <si>
     <t>Smartphone Motorola XT531 Spice XT, Desbloqueado, Titanio, Android 2.3, Processador 800MHZ, Tela Touch 3.5", Camera 5MP, 3G, Wi-Fi, Memoria Interna 150MB e Cartao de Memoria de 2GB</t>
   </si>
   <si>
-    <t>MOTOROLA SPICE XT</t>
+    <t>SPICE XT</t>
   </si>
   <si>
     <t>Smartphone Motorola RAZR Desbloqueado Tim, Preto - Android 2.3, Processador Dual Core, Tela Touch 4.3", Camera 8MP,Camera Frontal 1.3 MP,  3G, Wi-Fi e Memoria Interna de 16GB</t>
   </si>
   <si>
-    <t>MOTOROLA RAZR</t>
+    <t>RAZR</t>
   </si>
   <si>
     <t>Smartphone Motorola Fire. Preto. Dual Chip.  Touchscreen 2.8". Android 2.3. Cam 3MP. 3G. Wi Fi. GPS + Cartao Memoria 2GB</t>
@@ -988,7 +988,7 @@
     <t>Smartphone Motorola Milestone 3 Desbloqueado TIM Preto - Android 2.3, Processador Dual Core 1GHz, Tela 4", Camera 8MP, 3G, Wi-Fi e Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>MOTOROLA MILESTONE 3</t>
+    <t>MILESTONE 3</t>
   </si>
   <si>
     <t>Smartphone Motorola DEFY Desbloqueado Oi - Android 2.3 Wi Fi 3G Camera 5MP 2GB Cartao de Memoria 8GB</t>
@@ -1003,7 +1003,7 @@
     <t>Smartphone LG Optimus 3D P920  Desbloqueado Vivo Preto Camera 5.0MP 3G Wi Fi  Memoria Interna 8GB Cartao de Memoria 4GB</t>
   </si>
   <si>
-    <t>LG OPTIMUS 3 D</t>
+    <t>OPTIMUS 3 D</t>
   </si>
   <si>
     <t>Smartphone LG P970 Optimus Black Desbloqueado Tim, Preto - Android 2.2, Processador 1GHZ, Tela 4", Camera de 5MP, 3G, Wi-Fi e Memoria Interna 1GB</t>
@@ -1024,7 +1024,7 @@
     <t>Smartphone LG Opitmus 4x HD P880 Preto Android 4.0 3G Desbloqueado Vivo - Camera 8MP Wi-Fi GPS NFC e Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>LG OPITMUS 4 X HD</t>
+    <t>OPITMUS 4 X HD</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L5 E612 Branco - GSM. Android 4.0. Camera 5MP. 3G. Wi Fi. Memoria Interna de 4GB</t>
@@ -1033,13 +1033,13 @@
     <t>Smartphone Lg L Prime Plus Tv H502 Desbloqueado Branco</t>
   </si>
   <si>
-    <t>LG L PRIME PLUS TV</t>
+    <t>L PRIME PLUS TV</t>
   </si>
   <si>
     <t>Smartphone Lg L Prime Dual D337 Dual Chip Desbloqueado Android 4.4 Tela 5 8gb 3g - Preto</t>
   </si>
   <si>
-    <t>LG L PRIME DUAL</t>
+    <t>L PRIME DUAL</t>
   </si>
   <si>
     <t>Smartphone Lg L Prime Dual D337 Dual Chip Desbloqueado Android 4.4 Tela 5 8gb 3g - Branco</t>
@@ -1048,7 +1048,7 @@
     <t>Smartphone LG Prada P940H Preto Desbloqueado Vivo - GSM. Touchscreen. Tela 4.3". WVGA. Android 2.3. Processador Tri-DUAL 1.2GHz. Dualcore. WiFi. 3G. Camera 8MP. Filmadora. MP3 Player. Radio FM. Bluetooth. GPS. Fone de Ouvido. Cabo de Dados. Memoria Interna 8GB Expansivel</t>
   </si>
   <si>
-    <t>LG PRADA</t>
+    <t>PRADA</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto X (2a Geracao) Desbloqueado Android 4.4 Tela 5.2" 32GB 4G 13MP Wi-Fi</t>
@@ -1057,13 +1057,13 @@
     <t>Smartphone Motorola ATRIX Preto - GSM c/ Sistema Operacional Android 2.2, Processador Dual Core, Tecnologia 3G, Wi-Fi, TouchScreen c/ tela 4", Camera 5MP c/ zoom 8x, Filmadora HD, MP3 Player, Radio FM, Bluetooth 2.1, Fone, Cabo de Dados e Memoria Interna</t>
   </si>
   <si>
-    <t>MOTOROLA ATRIX</t>
+    <t>ATRIX</t>
   </si>
   <si>
     <t>Smartphone Motorola A1200i GSM Tim Quadri-band com Display Touch-screen colorido, MP3 Player, Radio FM, Camera 2.0MP c/ zoom 8x, Bluetooth,Fone e Cabo de Dados</t>
   </si>
   <si>
-    <t>MOTOROLA A1200I</t>
+    <t>A1200I</t>
   </si>
   <si>
     <t>Smartphone Motorola Spice Preto - GSM - Desbloqueado TIM  c/ Sistema Operacional Android 2.1, c/ Tecnologia 3G, Wi-Fi, GPS, TouchScreen,Teclado QWERTY, Camera 3.2MP c/ Zomm 8x, Filmadora, MP3 Player, Radio FM, Bluetooth, Fone, Cabo de Dados e Cartao 2GB</t>
@@ -1081,19 +1081,19 @@
     <t>Smartphone Nokia Lumia 930 Desbloqueado Windows 8.1 32GB 4G Wi-Fi Camera 20MP - Branco</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 930</t>
+    <t>LUMIA 930</t>
   </si>
   <si>
     <t>Smartphone LG G3 Desbloqueado Android 4.4 Kit Kat Tela 5.5" 16GB 4G Wi-Fi Camera 13MP - Titanio</t>
   </si>
   <si>
-    <t>LG G3</t>
+    <t>G3</t>
   </si>
   <si>
     <t>Smartphone LG Joy H222F Dual chip Desbloqueado Android 4.4 Kitkat Tela 4" 4GB 3G Wi-Fi Camera 5MP - Titanio</t>
   </si>
   <si>
-    <t>LG JOY</t>
+    <t>JOY</t>
   </si>
   <si>
     <t>Smartphone Motorola Novo Moto G (2a Geracao) Colors Dual Chip XT1068 Desbloqueado Android 5.0 Tela 5" 8GB 3G Wi-Fi Camera 8MP - Preto</t>
@@ -1108,7 +1108,7 @@
     <t>Smartphone Samsung Galaxy Win 2 Duos Dual Chip Desbloqueado Vivo Android 4.4 Tela 4.5" 8GB Wi-Fi Camera 5MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY WIN 2 DUOS</t>
+    <t>GALAXY WIN 2 DUOS</t>
   </si>
   <si>
     <t>Smartphone LG Optimus L5 II Preto - Android 4.1 3G Desbloqueado Camera 5MP Wi-Fi</t>
@@ -1117,13 +1117,13 @@
     <t>Smartphone Samsung Galaxy J1 Duos Dual Chip Desbloqueado Tim Android 4.4 Tela 4.3" 4GB 4G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY J1 DUOS</t>
+    <t>GALAXY J1 DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Mega 5.8 Duos Preto - GSM</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY MEGA 5.8 DUOS</t>
+    <t>GALAXY MEGA 5.8 DUOS</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L1 II Tri E475 Tri Chip Desbloqueado Android 4.1 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Rosa</t>
@@ -1132,7 +1132,7 @@
     <t>Smartphone Samsung Galaxy Ace 4 Duos Dual Chip Desbloqueado Android 4.4 Tela 4" 4GB 3G Camera 5MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE 4 DUOS</t>
+    <t>GALAXY ACE 4 DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Fame Lite S6790 Desbloqueado Vivo Android 4.1 Tela 3.5" 4GB Camera 3MP 3G Wi-Fi GPS - Preto</t>
@@ -1141,13 +1141,13 @@
     <t>Smartphone Motorola Moto Maxx Desbloqueado Android 4.4 Tela 5.2" Memoria 64GB Wi-Fi Camera 21MP Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO MAXX</t>
+    <t>MOTO MAXX</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E4 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 5MP - Branco</t>
   </si>
   <si>
-    <t>SONY XPERIA E4</t>
+    <t>XPERIA E4</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 800 Branco Windows Phone 7.5 3G Desbloqueado - Camera 8 MP com LED Flash, Tela 3.7", Processador 1.4GHz, Wi-Fi, GPS, Memoria interna de 16GB</t>
@@ -1159,19 +1159,19 @@
     <t>Smartphone Dual Chip Samsung Galaxy S Duos Desbloqueado Preto Android 4.0 Camera 5MP 3G Wi-Fi Memoria Interna de 3GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S DUOS</t>
+    <t>GALAXY S DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Ace 3 Desbloqueado Vivo 4G Cinza Android 4.2 Processador de 1.2 Ghz Dual Core</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE 3</t>
+    <t>GALAXY ACE 3</t>
   </si>
   <si>
     <t>Smartphone Xperia X8 Preto - GSM c/ Sistema Operacional Android 2.1, Tecnologia 3G, Wi-Fi, GPS, TouchScreen, Camera 3.2MP, Filmadora, MP3 Player, Radio FM, Bluetooth, Fone, Cabo de Dados e Cartao 2GB Desbloqueado Tim - Sony</t>
   </si>
   <si>
-    <t>SONY XPERIA X8</t>
+    <t>XPERIA X8</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z1 Desbloqueado Android 4.2 Tela 5" 16GB 4G Wi-Fi Camera 20MP - Roxo</t>
@@ -1180,19 +1180,19 @@
     <t>Smartphone Sony Xperia L Android 4.1 Tela 4.3" 8GB 3G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA L</t>
+    <t>XPERIA L</t>
   </si>
   <si>
     <t>Smartphone LG G2 Lite D295 Dual Chip Desbloqueado Android 4.4 Tela 4.5" 4GB 3G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>LG G2 LITE</t>
+    <t>G2 LITE</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Young Plus Dual Chip Desbloqueado Android 4.1 4GB 3G Wi-Fi Camera 3MP TV - Vermelho</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY YOUNG PLUS</t>
+    <t>GALAXY YOUNG PLUS</t>
   </si>
   <si>
     <t>Smartphone Positivo YPY S405 Dual Chip Desbloqueado Android 2.3 Tela 4" 3G Wi-Fi Camera 3MP - Preto</t>
@@ -1201,19 +1201,19 @@
     <t>Positivo</t>
   </si>
   <si>
-    <t>POSITIVO YPY</t>
+    <t>YPY</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 530 Desbloqueado Windows Phone 8.1 Tela 4" 4GB 3G Wi-Fi Camera 5MP GPS - Branco</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 530</t>
+    <t>LUMIA 530</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Young 2 Duos Dual Chip Desbloqueado Android 4.4 Tela 3.5" 4GB 3G Camera 3MP TV Digital - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY YOUNG 2 DUOS</t>
+    <t>GALAXY YOUNG 2 DUOS</t>
   </si>
   <si>
     <t>Smartphone LG G3 Beat Dual D724 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP - Branco</t>
@@ -1246,31 +1246,31 @@
     <t>Smartphone Sony Xperia M4 Aqua Dual Desbloqueado Android 5.0 Tela 5" Memoria Interna 16GB Camera de 13MP Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA M4 AQUA DUAL</t>
+    <t>XPERIA M4 AQUA DUAL</t>
   </si>
   <si>
     <t>Smartphone LG L20 D100 Android 4.4 4GB 3G Wi-Fi Camera 2MP - Preto e Grafite</t>
   </si>
   <si>
-    <t>LG L20</t>
+    <t>L20</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia M2 Aqua Desbloqueado Android 4.4 Tela 4.8" 8GB 4G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA M2 AQUA</t>
+    <t>XPERIA M2 AQUA</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia M2 Android 4.3 Tela 4.8" 8GB 4G Wi-Fi Camera 8MP GPS - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA M2</t>
+    <t>XPERIA M2</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Note III Branco Android 4.3 Camera de 13 MP Wi-Fi 4G Caneta S Pen</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY NOTE III</t>
+    <t>GALAXY NOTE III</t>
   </si>
   <si>
     <t>Smartphone LG G4 Desbloqueado Android 5.0 Tela 5.5" 32GB 4G Wi-Fi Camera 16MP Hexa Core - Titanio</t>
@@ -1294,7 +1294,7 @@
     <t>Smartphone Nokia Lumia 830 Desbloqueado Windows 8.1 Tela 5" 16GB Wi-Fi Camera 10MP GPS - Preto</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 830</t>
+    <t>LUMIA 830</t>
   </si>
   <si>
     <t>Smartphone Dual Chip LG Optimus L7 II Desbloqueado TIM Preto Android 4.1 3G/Wi Fi Camera 8MP 4GB</t>
@@ -1306,7 +1306,7 @@
     <t>Smartphone Samsung Galaxy Note 3 Neo Duos Dual Chip - Android 4.3 Tela 5.5" Camera 8MP com Caneta S Pen - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY NOTE 3 NEO DUOS</t>
+    <t>GALAXY NOTE 3 NEO DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A5 Dual Chip Desbloqueado Android 4.4 Tela 5" 16GB 4G Camera 13MP - Branco</t>
@@ -1315,13 +1315,13 @@
     <t>Smartphone Samsung Galaxy A5 Duos Dual Chip Desbloqueado Android 4.4 Tela 5" 16GB 4G Wi-Fi Camera 13MP - Dourado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A5 DUOS</t>
+    <t>GALAXY A5 DUOS</t>
   </si>
   <si>
     <t>Smartphone Positivo YPY S450 Dual-Chip Android 4.2 Tela 4" Wi-Fi Camera 5.0 MP - Preto</t>
   </si>
   <si>
-    <t>POSITIVO YPY DUAL CHIP</t>
+    <t>YPY DUAL CHIP</t>
   </si>
   <si>
     <t>Smartphone LG G3 Desbloqueado Vivo Android 4.4. Kit Kat Tela 5.5" 16GB 4G Camera 13MP Wi Fi - Titanio</t>
@@ -1330,7 +1330,7 @@
     <t>Smartphone Samsung Galaxy GT I9305 Desbloqueado Cinza Sistema Operacional Android 4.0 4G/Wi-Fi Camera 8MP Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GT</t>
+    <t>GALAXY GT</t>
   </si>
   <si>
     <t>Smartphone LG L20 D100 Android 4.4 4GB 3G Wi-Fi Camera 2MP - Branco</t>
@@ -1354,7 +1354,7 @@
     <t>Smartphone Sony Xperia T2 Ultra Dual Chip Desbloqueado Android 4.3 Tela 6" 8GB 3G 13MP Branco + Capa</t>
   </si>
   <si>
-    <t>SONY XPERIA T2 ULTRA</t>
+    <t>XPERIA T2 ULTRA</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia M2 Aqua Desbloqueado Claro Android 4.4 Tela 4.8" 8GB 4G Camera 8MP Preto</t>
@@ -1363,19 +1363,19 @@
     <t>Smartphone Samsung Galaxy Trend Lite Duos Dual Chip Desbloqueado Android 4.1 4GB 3G Wi-Fi Camera 3MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY TREND LITE DUOS</t>
+    <t>GALAXY TREND LITE DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S Duos 2 Dual Chip Desbloqueado Android 4.2 Tela 4" 4GB3G Wi-Fi Camera 5 MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S DUOS 2</t>
+    <t>GALAXY S DUOS 2</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy E5, 4g Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY E5</t>
+    <t>GALAXY E5</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Win 2 Duos Dual Chip Desbloqueado Android 4.4 Tela 4.5" 8GP 4G Camera 5MP - Cinza</t>
@@ -1396,7 +1396,7 @@
     <t>Smartphone LG F60 Dual Chip Desbloqueado Android 4.4 Tela 4.5" 4GB 4G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>LG F60</t>
+    <t>F60</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 Zoom 3G Desbloqueado Android 4.2 Tela 4.2" 8GB 3G Wi-Fi Camera 16MP GPS - Preto</t>
@@ -1405,7 +1405,7 @@
     <t>Smartphone LG OpTimus L4 II Dual TV Desbloqueado Tim Android 4.1 Tela 3.8" 4GB 3G Wi-Fi Camera 3MP - Branco</t>
   </si>
   <si>
-    <t>LG OPTIMUS L4 II DUAL TV</t>
+    <t>OPTIMUS L4 II DUAL TV</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E4 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 5MP - Preto</t>
@@ -1417,7 +1417,7 @@
     <t>Smartphone Nokia Lumia 920 Desbloqueado Branco 32GB - 4G Wi Fi Tela HD 4.5" Windows Phone 8 Camera 8.7MP Bluetooth GPS</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 920</t>
+    <t>LUMIA 920</t>
   </si>
   <si>
     <t>Smartphone LG L20 D100 Desbloqueado Vivo Android 4.4 4GB 3G Wi-Fi Camera 2MP - Branco</t>
@@ -1432,7 +1432,7 @@
     <t>Smartphone LG G Pro Lite Dual Chip Desbloqueado Android 4.1 Tela 5.5" 8GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>LG G PRO LITE</t>
+    <t>G PRO LITE</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy E5 E500m Duos Desbloqueado Preto</t>
@@ -1444,13 +1444,13 @@
     <t>Smartphone Samsung Galaxy S III Neo Duos Dual Chip Desbloqueado Android 4.3 Tela 4.8" 16GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S III NEO DUOS</t>
+    <t>GALAXY S III NEO DUOS</t>
   </si>
   <si>
     <t>Smartphone LG Optimus G Pro Desbloqueado Preto Android 4.1 4G Camera 13MP</t>
   </si>
   <si>
-    <t>LG OPTIMUS G PRO</t>
+    <t>OPTIMUS G PRO</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S6 G920i Desbloqueado Preto</t>
@@ -1471,7 +1471,7 @@
     <t>Smartphone Motorola Moto E 2a Geracao Tim Desbloqueado Android 5.0 Tela 4.5" 8GB 4G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO E</t>
+    <t>MOTO E</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto X 2a Geracao Desbloqueado Android 4.4 Tela 5.2" 32GB 4G Wi-Fi Camera 13MP GPS - Branco Bambu</t>
@@ -1507,7 +1507,7 @@
     <t>Smartphone Samsung Galaxy S4 Mini Duos Dual Chip Desbloqueado Android 4.2 Tela 4.3" 8GB 3G Wi-Fi Camera 8MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S4 MINI DUOS</t>
+    <t>GALAXY S4 MINI DUOS</t>
   </si>
   <si>
     <t>Smartphone LG G2 Lite D295 Dual Chip Desbloqueado Android 4.4 Tela 4.5" 4GB 3G Wi-Fi Camera 8MP - Branco</t>
@@ -1519,7 +1519,7 @@
     <t>Multilaser</t>
   </si>
   <si>
-    <t>MULTILASER TREND</t>
+    <t>TREND</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto G (2a Geracao) Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera de 8MP - Preto</t>
@@ -1528,7 +1528,7 @@
     <t>Smartphone Samsung Galaxy A7 A700 Duos Desbloqueado Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A7 DUOS</t>
+    <t>GALAXY A7 DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A7 A700 Duos Desbloqueado Dourado</t>
@@ -1537,13 +1537,13 @@
     <t>Smartphone Samsung Galaxy S3 Slim G3812 Dual Chip Desbloqueado Tim Android 4.2.2 Tela 4.5" 8GB 3G Wi-Fi Camera 5MP Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S3 SLIM</t>
+    <t>GALAXY S3 SLIM</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L4 II Dual TV Desbloquado Tim Preto Android 4.1 Tela 3.8" 4GB 3G Wi-Fi Camera de 3MP - Preto</t>
   </si>
   <si>
-    <t>LG OPTIMUS L4 II DUAL TV DESBLOQUADO</t>
+    <t>OPTIMUS L4 II DUAL TV DESBLOQUADO</t>
   </si>
   <si>
     <t>Smartphone Blu Studio 5.0 C Hd, Android 4.4, Dual Chip, Camera 8mp, Mem 4gb, Tela 5.0, 3g - Branco</t>
@@ -1558,7 +1558,7 @@
     <t>Smartphone Microsoft Lumia 435 Dual Chip Desbloqueado Windows Phone 8.1 Tela 4" 8GB 3G Wi-Fi Camera 2MP - Branco</t>
   </si>
   <si>
-    <t>MICROSOFT LUMIA 435</t>
+    <t>LUMIA 435</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Core Plus Dual Chip Desbloqueado Tim Android 4.3 Tela 4.3" 4GB 3G Wi-Fi Camera 5MP Preto</t>
@@ -1570,13 +1570,13 @@
     <t>Smartphone Asus ZenFone 5 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP Branco</t>
   </si>
   <si>
-    <t>ASUS ZENFONE 5</t>
+    <t>ZENFONE 5</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia C4 Selfie Dual Desbloqueado Android 5 Lollipop Tela Full HD 5.5" 16GB de Memoria Interna 4G Camera Frontal 5MP e Traseira 13MP Branco</t>
   </si>
   <si>
-    <t>SONY XPERIA C4 SELFIE DUAL</t>
+    <t>XPERIA C4 SELFIE DUAL</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A3 Duos Dual Chip Desbloqueado Android 4.4 Tela Super Amoled 4.5" 16GB Wi-Fi 4G Camera 8MP - Dourado</t>
@@ -1585,7 +1585,7 @@
     <t>Smartphone LG D157 TV L35 Dual Chip Desbloqueado Android 4.4 Tela 3.2" 4GB 3G Wi-Fi Camera 3MP TV Digital - Preto</t>
   </si>
   <si>
-    <t>LG TV L35</t>
+    <t>TV L35</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Note 4 Desbloqueado Android 4.4 Tela 5.7" 32GB Wi-Fi Camera de 16MP - Branco</t>
@@ -1597,7 +1597,7 @@
     <t>Smartphone LG G2 Mini D618 Dual Chip Desbloqueado Android 4.4 Tela 4.7" 8GB 3G Wi-Fi 8MP - Branco</t>
   </si>
   <si>
-    <t>LG G2 MINI</t>
+    <t>G2 MINI</t>
   </si>
   <si>
     <t>Smartphone LG G2 Mini D618 Dual Chip Desbloqueado Android 4.4 Tela 4.7" 8GB 3G Wi-Fi 8MP - Preto</t>
@@ -1606,7 +1606,7 @@
     <t>Smartphone Motorola Moto G Colors Edition Dual Chip Desbloqueado Android 4.3 Tela 4.5" 16GB 3G Wi-Fi Camera 5MP GPS - Preto</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO G COLORS EDITION</t>
+    <t>MOTO G COLORS EDITION</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L7 II Desbloqueado Android 4.1 Tela 4.3" 4GB 3G Wi-Fi - Camera 8MP - Branco</t>
@@ -1624,7 +1624,7 @@
     <t>Smartphone LG Volt H422TV Dual Chip Desbloqueado Android 5.0 Tela 4.7" 8GB 3G Wi-Fi Camera 8MP com TV Digital - Dourado</t>
   </si>
   <si>
-    <t>LG VOLT</t>
+    <t>VOLT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy E5 Duos Dual Chip Desbloqueado Android 4.4 Tela Amoled HD 5" 16GB 4G Wi-Fi Camera 8MP - Branco</t>
@@ -1648,13 +1648,13 @@
     <t>Smartphone LG OpTimus 3D Max P720H Android 2.3 Tela 4.3" 3G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>LG OPTIMUS 3 D MAX</t>
+    <t>OPTIMUS 3 D MAX</t>
   </si>
   <si>
     <t>Smartphone Dual Chip LG Optimus L5 II Dual Branco Android 4.1 Desbloqueado - Camera 5.0MP 3G Wi-Fi GPS</t>
   </si>
   <si>
-    <t>LG OPTIMUS L5 II DUAL</t>
+    <t>OPTIMUS L5 II DUAL</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L5 II Dual Chip Desbloqueado Android 4.1 Tela 4" 4GB 3G Wi-Fi Camera 5MP - Preto</t>
@@ -1669,7 +1669,7 @@
     <t>Smartphone LG L Prime D337 Dual Chip Android 4.4 Kit Kat Tela 5" 8GB 3G Wi-Fi Camera 8MP - Dourado</t>
   </si>
   <si>
-    <t>LG L PRIME</t>
+    <t>L PRIME</t>
   </si>
   <si>
     <t>Smartphone LG L Prime Dual D337 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP TV Digital - Branco</t>
@@ -1690,13 +1690,13 @@
     <t>Smartphone Motorola Moto E DTV Colors Dual Chip Desbloqueado Android 4.4 Tela 4.3" 4GB 3G Wi-Fi Camera 5MP GPS TV Digital - Branco</t>
   </si>
   <si>
-    <t>MOTOROLA MOTO E DTV COLORS</t>
+    <t>MOTO E DTV COLORS</t>
   </si>
   <si>
     <t>Smartphone LG L40 D175 Dual Chip Desbloqueado Android 4.4 Tela 3.5" 4GB 3G Wi-Fi Camera 3MP - Rosa</t>
   </si>
   <si>
-    <t>LG L40</t>
+    <t>L40</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L1 II Desbloqueado Android 4.1 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Branco</t>
@@ -1708,7 +1708,7 @@
     <t>Smartphone LG L50 Sporty TV Dual Chip Desbloqueado Android 4.4 Kit Kat Tela 4" 4GB 3G Wi-Fi Camera 5MP - Branco e Rosa</t>
   </si>
   <si>
-    <t>LG L50 SPORTY TV</t>
+    <t>L50 SPORTY TV</t>
   </si>
   <si>
     <t>Smartphone LG D375 L80 Desbloqueado Android 4.4 Kitkat Tela 5'' 8GB Wi-Fi Camera de 8MP TV Digital - Preto</t>
@@ -1717,7 +1717,7 @@
     <t>Smartphone Samsung Galaxy Gran Prime Duos Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP TV Digital - Cinza</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN PRIME DUOS</t>
+    <t>GALAXY GRAN PRIME DUOS</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z1 Desbloqueado Android 4.2 Tela 5" 16GB 4G Wi-Fi Camera 20MP - Branco</t>
@@ -1732,13 +1732,13 @@
     <t>Smartphone Dual Chip Nokia X Desbloqueado Preto Nokia Platform 1.1 Conexao 3G Memoria Interna 4GB</t>
   </si>
   <si>
-    <t>NOKIA X</t>
+    <t>X</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E Dual Chip Desbloqueado Tim Preto Android 4.0 3G Wi-Fi Camera 3.2MP - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA E</t>
+    <t>XPERIA E</t>
   </si>
   <si>
     <t>Smartphone Asus Zenfone 6 Dual Chip Desbloqueado Android 4.4 Tela 6" 32GB 3G Camera 13MP - Branco</t>
@@ -1747,7 +1747,7 @@
     <t>Smartphone Positivo X800 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 13MP - Preto</t>
   </si>
   <si>
-    <t>POSITIVO X800</t>
+    <t>X800</t>
   </si>
   <si>
     <t>Smartphone LG L50 Dual Chip Desbloqueado Tim Android 4.4 Tela 4" 4GB Wi-Fi 3G Camera 5MP com TV Digital - Branco e Rosa</t>
@@ -1762,19 +1762,19 @@
     <t>Smartphone LG G3 Beat Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP - Dourado</t>
   </si>
   <si>
-    <t>LG G3 BEAT</t>
+    <t>G3 BEAT</t>
   </si>
   <si>
     <t>Smartphone Alcatel Pop C7 Dualchip 704B Desbloqueado Android 4.2 Tela 5" 4GB Micro SD ate 32GB Camera de 5MP GPS - Branco</t>
   </si>
   <si>
-    <t>ALCATEL POP C7 DUALCHIP 704 B</t>
+    <t>POP C7 DUALCHIP 704 B</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia T3 Desbloqueado Android 4.4 Tela 5.3" 8GB 4G Wi-Fi Camera de 8MP - Branco</t>
   </si>
   <si>
-    <t>SONY XPERIA T3</t>
+    <t>XPERIA T3</t>
   </si>
   <si>
     <t>Smartphone Alcatel OT-4007E Pixi Dual Chip Desbloqueado Claro Android 2.3 Tela 3.5" 100MB 3G Wi-Fi Camera 2MP - Preto</t>
@@ -1789,7 +1789,7 @@
     <t>Smartphone Multilaser MS2 Android 4.2 Wi Fi Bluetooth Camera 3.0 MP 4GB Cartao Micro SD GPS Dual Chip - Azul</t>
   </si>
   <si>
-    <t>MULTILASER MS2</t>
+    <t>MS2</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Trend Lite Duos Dual Chip Desbloqueado Android 4.1 4GB 3G Wi-Fi Camera 3MP - Preto</t>
@@ -1801,7 +1801,7 @@
     <t>Smartphone Samsung Galaxy Gran Duos Desbloqueado Vivo - Dual Chip Tela 5" Android 4.1 Camera 8MP 3G Wi-Fi Bluetooth GPS</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN DUOS</t>
+    <t>GALAXY GRAN DUOS</t>
   </si>
   <si>
     <t>Smartphone LG Joy H222F Dual Chip Desbloqueado Android 4.4 Kitkat Tela 4" 4GB 3G Wi-Fi Camera 5MP- Branco</t>
@@ -1846,13 +1846,13 @@
     <t>Smartphone Sony Xperia Z2 Desbloqueado Android 4.4 Tela 5.2" 16GB 4G Wi-Fi Camera 20.7MP GPS TV Digital - Branco + Pulseira SmartBand</t>
   </si>
   <si>
-    <t>SONY XPERIA Z2</t>
+    <t>XPERIA Z2</t>
   </si>
   <si>
     <t>Smartphone Multilaser MS4 Dual Chip Android 4.2 Tela 4.5" 4GB 3G Wi-Fi Camera 8MP - Branco</t>
   </si>
   <si>
-    <t>MULTILASER MS4</t>
+    <t>MS4</t>
   </si>
   <si>
     <t>Smartphone LG G4 Desbloqueado Android 5.1 Lollipop Tela 5,5'' 32GB Wi-Fi Camera de 16MP - Couro Preto</t>
@@ -1861,7 +1861,7 @@
     <t>Smartphone Samsung Galaxy Pocket Plus Duos Desbloqueado Tim Branco Android 4.0 Camera 2MP Memoria Interna 3GB Wi Fi GPS</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY POCKET PLUS DUOS</t>
+    <t>GALAXY POCKET PLUS DUOS</t>
   </si>
   <si>
     <t>Smartphone LG G4 Desbloqueado Android 5.1 Lollipop Tela 5,5'' 32GB Wi-Fi Camera de 16MP - Titanio</t>
@@ -1870,7 +1870,7 @@
     <t>Smartphone Samsung Galaxy Note II Desbloqueado Tim Cinza Android 4.1 Camera de 8.0MP 3G Wi Fi Memoria Interna de 16GB + Caneta S Pen</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY NOTE II</t>
+    <t>GALAXY NOTE II</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Fame Duos Dual Chip Desbloqueado Android 4.1 Tela 3.5" 4GB Camera 5MP 3G Wi-Fi GPS - Grafite</t>
@@ -1885,7 +1885,7 @@
     <t>Smartphone LG G Flex2 Desbloqueado Android 5.0 Tela 5.5" 16GB 4G Camera 13MP e Processador Octa Core - Titanio</t>
   </si>
   <si>
-    <t>LG G</t>
+    <t>G</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S III I9300 Desbloqueado Android 4.0 Tela 4.8" 16GB 3G Wi-Fi Camera 8MP GPS - Branco</t>
@@ -1894,7 +1894,7 @@
     <t>Smartphone Samsung Galaxy Alpha Desbloqueado Android 4.4 Tela 4.7" 32GB 4G Wi-Fi Camera 12MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ALPHA</t>
+    <t>GALAXY ALPHA</t>
   </si>
   <si>
     <t>Smartphone LG Joy H222F Dual chip Desbloqueado Android 4.4 Kitkat Tela 4" 4GB 3G Wi-Fi Camera 5MP- Azul</t>
@@ -1921,19 +1921,19 @@
     <t>Smartphone Sony Ericsson Xperia  arc 3G Android 2.3 Wi-Fi Cam 8MP aGPS 16GB</t>
   </si>
   <si>
-    <t>SONY XPERIA ARC</t>
+    <t>XPERIA ARC</t>
   </si>
   <si>
     <t>Smartphone Sony Ericsson Xperia neo 3G Android 2.3 Wi Fi Cam 8.1MP aGPS 8GB - Desbloqueado Claro</t>
   </si>
   <si>
-    <t>SONY XPERIA NEO</t>
+    <t>XPERIA NEO</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Gran Prime Duos Sm-G531b 5 8gb Android 4-4 8mp Tv Quad Core Dourado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN PRIME DUOS SM 5</t>
+    <t>GALAXY GRAN PRIME DUOS SM 5</t>
   </si>
   <si>
     <t>Smartphone LG G4 Desbloqueado Android 5.1 Lollipop Tela 5,5'' 32GB Wi-Fi Camera de 16MP - Branco</t>
@@ -1948,7 +1948,7 @@
     <t>Huawei</t>
   </si>
   <si>
-    <t>HUAWEI ASCEND</t>
+    <t>ASCEND</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E1 Dual Chip Desbloqueado Android 4.3 Tela 4" 3G Wi-Fi Camera 3MP TV Digital - Branco</t>
@@ -1969,19 +1969,19 @@
     <t>Smartphone Nokia Lumia 1020 Smartphone Desbloqueado Windows Phone 8 Tela 4.5" 32GB 4G Wi-Fi Camera 41MP GPS - Branco</t>
   </si>
   <si>
-    <t>NOKIA LUMIA</t>
+    <t>LUMIA</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Core 2 Duos G355M Dual Chip Android 4.4 Tela 4.5" 3G Wi-Fi Camera 5MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY CORE 2 DUOS</t>
+    <t>GALAXY CORE 2 DUOS</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 730 Desbloqueado Tela 4.7 Dual Chip 3g Windows Phone 8 Laranja</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 730</t>
+    <t>LUMIA 730</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia E Dual Chip Desbloqueado Claro Android 4.0 Tela 3.5" 3G Wi-Fi Camera 3.2MP - Preto</t>
@@ -1990,13 +1990,13 @@
     <t>Smartphone Samsung Omnia M, Desbloqueado, Preto, Tela Super Amoled 4", Touchscreen, Processador 1Ghz, Windows Phone 7.5, Camera 5MP, 3G, Wi-Fi e Memoria Interna 4GB</t>
   </si>
   <si>
-    <t>SAMSUNG OMNIA M</t>
+    <t>OMNIA M</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Ace - Branco -  GSM, Tela Touch 3.5", Android 2.2, Processador 800 MHz, 3G, Wi-Fi, GPS,Camera de 5MP, Incluso cartao de memoria de 2GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE</t>
+    <t>GALAXY ACE</t>
   </si>
   <si>
     <t>Smartphone LG G3 Desbloqueado Android 4.4 Kit Kat Tela 5.5" 16GB 4G Wi-Fi Camera 13MP - Branco</t>
@@ -2014,7 +2014,7 @@
     <t>Smartphone Alcatel Idol Dual Chip Desbloqueado Android 4.1 Tela 4.7" 16GB 3G Wi-Fi Camera 8MP - Cinza</t>
   </si>
   <si>
-    <t>ALCATEL IDOL</t>
+    <t>IDOL</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 Mini Dual Chip 3g 8gb Dual Core 1,7ghz | Cor: Preto</t>
@@ -2023,19 +2023,19 @@
     <t>Smartphone Samsung Galaxy Core Ii Duos, 3g Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY CORE II DUOS</t>
+    <t>GALAXY CORE II DUOS</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia C Dual Chip Desbloqueado Android 4.2 Tela 5" 4GB 3G Wi-Fi Camera 8MP - Roxo</t>
   </si>
   <si>
-    <t>SONY XPERIA C</t>
+    <t>XPERIA C</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Music Duos Dual Chip Desbloqueado Android 4.0 Tela 3" Wi-Fi 4GB Camera 3.2MP GPS - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY MUSIC DUOS</t>
+    <t>GALAXY MUSIC DUOS</t>
   </si>
   <si>
     <t>Smartphone LG OpTimus L7 II Dual Chip Desbloqueado Tim Android 4.1 Tela 4.3" 4GB 3G Wi-Fi Camera 8MP - Branco</t>
@@ -2047,7 +2047,7 @@
     <t>Smartphone Samsung Galaxy Y Prata Desbloqueado Claro - GSM, Android 2.3, Processador 832MHz, Camera de 2MP, 3G, Wi-Fi, Touchscreen 3", Teclado Swype, Cartao de Memoria 2GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY Y</t>
+    <t>GALAXY Y</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy SIII 4G Desbloqueado Prata</t>
@@ -2059,7 +2059,7 @@
     <t>Smartphone Positivo YPYS460 TV Dual Chip Desbloqueado Android 4.2 Tela 4" 3G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>POSITIVO TV</t>
+    <t>TV</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A3 4g Duos, Sm-A300m/Ds, Quad Core 1.2 Ghz, Camera 8 Mp, Branco</t>
@@ -2077,7 +2077,7 @@
     <t>Smartphone Galaxy S5 Mini Desbloqueado Branco / Dual Chips / CaMera De 8.0 Mp / Flash / Tela 4.5</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S5 MINI</t>
+    <t>GALAXY S5 MINI</t>
   </si>
   <si>
     <t>Smartphone Dual Chip Nokia X Desbloqueado Branco Nokia Platform 1.1 Conexao 3G Memoria Interna 4GB</t>
@@ -2101,19 +2101,19 @@
     <t>Smartphone Nokia Lumia 925 Desbloqueado Branco Memoria Interna 16 GB - 4G Wi-Fi Tela HD 4.5" Windows Phone 8 Camera 8.7MP Bluetooth GPS</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 925</t>
+    <t>LUMIA 925</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Gran Neo Duos Dual Chip Desbloqueado Android 4.2 Tela 5" 8GB 3G Wi-Fi Camera 5MP TV Digital - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN NEO DUOS</t>
+    <t>GALAXY GRAN NEO DUOS</t>
   </si>
   <si>
     <t>SmartphoneTri Chip Samsung Galaxy Star Trios Desbloqueado Android 4.1 Wi-Fi,3G Camera 2MP Memoria Interna 4GB GPS</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY STAR TRIOS</t>
+    <t>GALAXY STAR TRIOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Duos SM-G900M Dual Chip Desbloqueado Android 4.4 Tela 5.1" 16GB 4G Wi-Fi GPS - Azul</t>
@@ -2122,7 +2122,7 @@
     <t>Smartphone Samsung Galaxy S II Duos S7273 Dual Chip Desbloqueado Tim Android 4.2 4GB TV Digital - Cinza</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S II DUOS</t>
+    <t>GALAXY S II DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S4 Mini Duos Dual Chip Desbloqueado Android 4.2 Tela 4.3" 8GB 3G Wi-Fi Camera 8MP - Rosa</t>
@@ -2131,7 +2131,7 @@
     <t>Smartphone Sony Xperia Z3 Desbloqueado Android 4.4 Tela 5.2" 16GB 4G Wi-Fi Camera 20.7MP - Preto + Pulseira SmartBand</t>
   </si>
   <si>
-    <t>SONY XPERIA Z3</t>
+    <t>XPERIA Z3</t>
   </si>
   <si>
     <t>Smartphone Alcatel Idol Dual Chip Desbloqueado Android 4.1 Tela 4.7" 16GB 3G Wi-Fi Camera de 8MP - Prata</t>
@@ -2146,31 +2146,31 @@
     <t>Smartphone Nokia C3 Desbloqueado Claro, Dourado / Branco - Symbian S40 6.0, Camera 2.0MP, Wi-Fi, Camera 2.0MP, Memoria Interna 55MB e Cartao 2GB</t>
   </si>
   <si>
-    <t>NOKIA C3</t>
+    <t>C3</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Young Duos Dual Chip Desbloqueado Android 4.1 Tela 3.2" 3G Wi-Fi Camera 3MP 4GB GPS TV Digital - Prata</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY YOUNG DUOS</t>
+    <t>GALAXY YOUNG DUOS</t>
   </si>
   <si>
     <t>Smartphone Multilaser MS5 Android 4.2 Wi Fi Bluetooth Camera 8.0 MP 4GB Cartao Micro SD GPS - Branco</t>
   </si>
   <si>
-    <t>MULTILASER MS5</t>
+    <t>MS5</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 900 Preto - GSM Tela Curva 4.3" AMOLED Windows Phone 7.5 Processador 1.4GHz 3G Wi Fi GPS Camera 8 MP Camera Frontal de 1.3 MP MP3 Player Memoria interna de 16GB e Gratis 25GB de Armazenamento no Sky Drive - Desbloqueado Vivo</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 900</t>
+    <t>LUMIA 900</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Trend Lite S7390 Desbloqueado Claro Android 4.2 Tela 4" 4GB 3G Wi-Fi Camera 3MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY TREND LITE</t>
+    <t>GALAXY TREND LITE</t>
   </si>
   <si>
     <t>Smartphone LG E400f Optimus L3 Desbloqueado Oi BrancoAndroid 2.3 3G Wi-Fi Camera 3.2MP Memoria interna de 2 GB</t>
@@ -2179,7 +2179,7 @@
     <t>Smartphone Nokia N8 Desbloqueado Claro, Cinza - Symbian 3, Tela 3.5", Camera 12MP, 3G, Wi-Fi e Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>NOKIA N8</t>
+    <t>N8</t>
   </si>
   <si>
     <t>Smartphone LG G2 Desbloqueado Android 4.2 Jely Bean Tela 5.2" 16GB 4G Wi-Fi Camera 13MP - Dourado</t>
@@ -2191,13 +2191,13 @@
     <t>Smartphone Sony Xperia Z Ultra Desbloqueado Android 4.2 Tela 6.4" 16GB 4G Wi-Fi Camera 8MP GPS TV Digital - Preto</t>
   </si>
   <si>
-    <t>SONY XPERIA Z ULTRA</t>
+    <t>XPERIA Z ULTRA</t>
   </si>
   <si>
     <t>Smartphone Nokia X3-02 Desbloqueado Azul Camera 5MP 3G Wi-Fi Cartao 2GB</t>
   </si>
   <si>
-    <t>NOKIA X3</t>
+    <t>X3</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia L Android 4.1 Tela 4.3" 8GB 3G Wi-Fi Camera 8MP GPS - Branco</t>
@@ -2209,7 +2209,7 @@
     <t>Smartphone Alcatel Pop C7 Dualchip 704BR Desbloqueado Android 4.2 Tela 5" 4GB Camera de 5MP GPS - Branco</t>
   </si>
   <si>
-    <t>ALCATEL POP C7 DUALCHIP 704 BR</t>
+    <t>POP C7 DUALCHIP 704 BR</t>
   </si>
   <si>
     <t>Smartphone Sony Ericsson Xperia Arc S Desbloqueado Tim Prata Android 2.3 Camera 8MP 3G Wi-Fi Memoria Interna 320MB Cartao 16 GB</t>
@@ -2224,13 +2224,13 @@
     <t>Smartphone Nokia C7-00 Prata Symbian3 Wi Fi 3G Cam 8MP GPS MP3 FM 8GB</t>
   </si>
   <si>
-    <t>NOKIA C7</t>
+    <t>C7</t>
   </si>
   <si>
     <t>Smartphone Dual Chip Samsung Galaxy Young Duos TV, Desbloqueado, Vermelho, Android 4.1, Processador 1Ghz, Tela 3.2", Camera 3MP, 3G, Wi-Fi, GPS e Memoria Interna 4GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY YOUNG DUOS TV</t>
+    <t>GALAXY YOUNG DUOS TV</t>
   </si>
   <si>
     <t>Smartphone Huawei Ascend G510 Desbloqueado Preto Android 4.1 3G/Wi Fi Camera 5MP 4GB</t>
@@ -2242,25 +2242,25 @@
     <t>Smartphone Samsung Galaxy Y TV Desbloqueado Claro S5367 Prata - GSM, Camera 3.2MP, Touchscreen, 3G, Wi-Fi, Memoria interna 180MB, Cartao de Memoria 2GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY Y TV</t>
+    <t>GALAXY Y TV</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S III I9300 Metallic Blue Android 4.0 3G - Camera 8MP Wi-Fi GPS Memoria Interna 16GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S III METALLIC BLUE</t>
+    <t>GALAXY S III METALLIC BLUE</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Ace Duos S6802 Dual Chip Preto Tela Touch 3.5" - Android 2.3 3G WiFi Camera 5MP Memoria Interna de 3GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE DUOS</t>
+    <t>GALAXY ACE DUOS</t>
   </si>
   <si>
     <t>Smartphone Nokia Asha 311 Desbloqueado Vivo Tela 3" 256MB 3G Wi-Fi Camera de 3.2MP - Preto</t>
   </si>
   <si>
-    <t>NOKIA ASHA 311</t>
+    <t>ASHA 311</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 820, Desbloqueado TIM, Preto, Windows Phone 8, 4G, Wi-Fi, Camera 8MP, Memoria Interna 8GB, GPS</t>
@@ -2272,7 +2272,7 @@
     <t>Smartphone Samsung Galaxy Fame GT-S6810 Desbloqueado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY FAME GT</t>
+    <t>GALAXY FAME GT</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia ZQ Desbloqueado Tim Preto Processador Quad-Core 1.5 Ghz Android 4.1 Tela 5" 4G Wi-Fi Camera 13MP Memoria Interna 16GB GPS NFC</t>
@@ -2287,7 +2287,7 @@
     <t>Smartphone Alcatel One Touch Idol Mini Dual Core Desbloqueado Android 4.2 Tela 4.3" 8GB 3G 5MP - Rosa</t>
   </si>
   <si>
-    <t>ALCATEL ONE TOUCH IDOL MINI</t>
+    <t>ONE TOUCH IDOL MINI</t>
   </si>
   <si>
     <t>Smartphone LG L40 D175 Dual Chip Desbloqueado Android 4.4 Tela 3.5" 4GB 3G Wi-Fi Camera 3MP - Branco</t>
@@ -2299,13 +2299,13 @@
     <t>Smartphone Positivo S550 Dual Chip Desbloqueado Android 4.4 Tela 5.5" 4GB 3G Wi-Fi Camera 5MP - Branco</t>
   </si>
   <si>
-    <t>POSITIVO S550</t>
+    <t>S550</t>
   </si>
   <si>
     <t>Smartphone Huawei Ascend Y330 Colors Desbloqueado Tela 4 3g Android 4.2 Preto</t>
   </si>
   <si>
-    <t>HUAWEI ASCEND COLORS</t>
+    <t>ASCEND COLORS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Gran Prime Duos Desbloqueado Android 4.4 Tela 5" 8GB 3G Camera 8MP TV Digital - Dourado</t>
@@ -2314,7 +2314,7 @@
     <t>Smartphone Alcatel M Pop Dual Chip Desbloqueado Android 4.1 Tela 4" 4GB 3G Wi-Fi Camera de 5MP - Preto</t>
   </si>
   <si>
-    <t>ALCATEL M POP</t>
+    <t>M POP</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia C Desbloqueado Android 4.2 Tela 5" 4GB 3G Wi-Fi Camera 8MP - Preto</t>
@@ -2329,7 +2329,7 @@
     <t>Smartphone Samsung Galaxy S4 Active Desbloqueado Android 4.2 Tela 5" 16GB 4G WiFi Camera de 8MP - Grafite</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY S4 ACTIVE</t>
+    <t>GALAXY S4 ACTIVE</t>
   </si>
   <si>
     <t>Smartphone Alcatel M Pop Dual Chip Desbloqueado Android 4.1 Tela 4" 512MB 3G Wi-Fi Camera 5MP - Roxo</t>
@@ -2341,7 +2341,7 @@
     <t>Smartphone Samsung Galaxy Gran Duos GT-I9082 Grafite Desbloqueado - GSM</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN DUOS GT</t>
+    <t>GALAXY GRAN DUOS GT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Gran Neo Duos Dual Chip Desbloqueado Android 4.2 3G Wi-Fi Camera 5MP TV Digital - Branco</t>
@@ -2353,13 +2353,13 @@
     <t>Smartphone Samsung Galaxy Pocket Plus Desbloqueado Tim Branco Android 4.0 Camera 2MP Memoria Interna 3GB Wi-Fi GPS</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY POCKET PLUS</t>
+    <t>GALAXY POCKET PLUS</t>
   </si>
   <si>
     <t>Smartphone Samsung Express Desbloqueado Vivo Cinza Android 4.1 4G Camera 5MP</t>
   </si>
   <si>
-    <t>SAMSUNG EXPRESS</t>
+    <t>EXPRESS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S III Branco 3G Desbloqueado Vivo - Camera 8MP Wi-Fi GPS 16GB</t>
@@ -2368,7 +2368,7 @@
     <t>Smartphone Samsung Galaxy Pocket Neo S5310 Branco - GSM</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY POCKET NEO</t>
+    <t>GALAXY POCKET NEO</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S II Desbloqueado VIVO, Preto - Android 2.3, Processador Dual Core, Tela Touch 4.27", Camera 8MP, 3G, Wi-Fi e Memoria Interna de 16GB</t>
@@ -2377,19 +2377,19 @@
     <t>Smartphone Samsung Galaxy SII Duos TV Cinza Desbloqueado Tim GSM</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY SII DUOS TV CINZA</t>
+    <t>GALAXY SII DUOS TV CINZA</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 625, Desbloqueado TIM, Preto, Processador 1.2GHz dual core ,Tela Touchscreen 4.7", Windows Phone 8, Camera 5MP com flash LED, Camera Frontal VGA, 4G, Wi-Fi, Bluetooth, GPS e Memoria Interna de 8G</t>
   </si>
   <si>
-    <t>NOKIA LUMIA 625</t>
+    <t>LUMIA 625</t>
   </si>
   <si>
     <t>Smartphone Huawei Ascend P6 Desbloqueado Rosa Android 4.2 3G/Wi Fi Camera 8 MP 8GB</t>
   </si>
   <si>
-    <t>HUAWEI ASCEND P6</t>
+    <t>ASCEND P6</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia ZQ Desbloqueado Claro Android 4.1 Tela 5" 16GB 4G Wi-Fi Camera 13MP - Vermelho</t>
@@ -2404,7 +2404,7 @@
     <t>Smartphone Positivo S450 Dual Chip Desbloqueado Android 4.2 Tela 4" Memoria interna 4GB ROM 3G Camera 5MP + Cartao 8GB - Branco</t>
   </si>
   <si>
-    <t>POSITIVO S450</t>
+    <t>S450</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy S5 Desbloqueado Android 4.4.2 Tela 5.1" 16GB 4G Wi-Fi Camera 16 MP - Azul</t>
@@ -2425,7 +2425,7 @@
     <t>Smartphone Samsung Galaxy Ace Plus Preto - Android 2.3 Processador 1GHz Tela Touchscreen 3.7" Camera 5.0MP 3G Wi-Fi Memoria Interna 3GB Expansivel ate 32GB</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE PLUS</t>
+    <t>GALAXY ACE PLUS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A7 A700 Duos Desbloqueado Branco</t>
@@ -2443,19 +2443,19 @@
     <t>Smartphone Nokia Asha 302 Desbloqueado TIM Branco - GSM Sistema Operacional S40 Asha Processador 1GHz 3G Wi Fi Camera 3.2 MP</t>
   </si>
   <si>
-    <t>NOKIA ASHA 302</t>
+    <t>ASHA 302</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Pocket 2 Duos G110b Desbloqueado Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY POCKET 2 DUOS</t>
+    <t>GALAXY POCKET 2 DUOS</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy SIII GT-I9300 Desbloqueado</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY SIII GT</t>
+    <t>GALAXY SIII GT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Note 3 Neo Duos Dual Chip Android 4.3 Tela 5.5" 16GB 3G Wi-Fi Camera de 8MP com Caneta S Pen - Branco</t>
@@ -2476,19 +2476,19 @@
     <t>Smartphone Samsung Galaxy Ace 4 Lite Duos Dual Chip Desbloqueado Android 4.4 Tela 4" 4GB 3G Wi-Fi Camera 3MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY ACE 4 LITE DUOS</t>
+    <t>GALAXY ACE 4 LITE DUOS</t>
   </si>
   <si>
     <t>Smartphone Alcatel POP 2 Single Chip Desbloqueado Android 4.4 Tela 4.5" Memoria Interna 8GB 4G Camera 5MP Branco</t>
   </si>
   <si>
-    <t>ALCATEL POP 2 SINGLE CHIP</t>
+    <t>POP 2 SINGLE CHIP</t>
   </si>
   <si>
     <t>Smartphone Multilaser MS1  Dual Chip Android 2.3 Tela 3.5" 512MB 3G Wi-Fi Camera 2MP - Branco e Rosa</t>
   </si>
   <si>
-    <t>MULTILASER MS1</t>
+    <t>MS1</t>
   </si>
   <si>
     <t>Smartphone LG L20 D100 Desbloqueado Vivo Android 4.4 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Preto e Grafite</t>
@@ -2497,19 +2497,19 @@
     <t>Smartphone Dual Chip Positivo S440 Desbloqueado Android 4.4 Tela 4" 4GB 3G Wi-Fi Camera 5.0 - Preto</t>
   </si>
   <si>
-    <t>POSITIVO S440</t>
+    <t>S440</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Core 2 Desbloqueado Claro Android 4.4 Tela 4.5" 4GB 3G Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY CORE 2</t>
+    <t>GALAXY CORE 2</t>
   </si>
   <si>
     <t>Smartphone Positivo S400 GSM Desbloqueado Dual Chip Android 4.0 Tela 4" 4GB 3G Wi-Fi Camera 5MP - Preto + Cartao de 8GB</t>
   </si>
   <si>
-    <t>POSITIVO S400</t>
+    <t>S400</t>
   </si>
   <si>
     <t>Smartphone LG Triple L20 D107 Android 4.4 Tela 3" 4GB 3G Wi-Fi Camera 2MP - Preto e Grafite</t>
@@ -2548,13 +2548,13 @@
     <t>Smartphone Samsung Galaxy Pocket 2 G110b Preto 4gb, Wi-Fi, Gps, Camera 2mp, 3g, Android 4.4 Kit-Kat</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY POCKET 2</t>
+    <t>GALAXY POCKET 2</t>
   </si>
   <si>
     <t>Smartphone Sony Ericsson Xperia Neo V Desbloqueado Tim, Prata, Android 2.3, Tela 3.7", Camera de 5MP, 3G, Wi-Fi, Memoria Interna 320MB e Cartao de Memoria 2GB</t>
   </si>
   <si>
-    <t>SONY XPERIA NEO V</t>
+    <t>XPERIA NEO V</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia M2 Aqua Desbloqueado Android 4.4, Tela 4,8 Mem. 8gb Camera De 8mp</t>
@@ -2563,7 +2563,7 @@
     <t>Smartphone Positivo S350 GSM Desbloqueado Preto Android 2.3 Dual Chip Tela Touchscreen 3.5" Camera de 3MP 3G Wi Fi Memoria interna 512MB Cartao de 2GB</t>
   </si>
   <si>
-    <t>POSITIVO S350</t>
+    <t>S350</t>
   </si>
   <si>
     <t>Smartphone Positivo X800 Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 13MP - Branco</t>
@@ -2578,7 +2578,7 @@
     <t>Smartphone Multilaser Connect Dual Chip Branco e rosa. Camera de 3MP. 3G. WIFI</t>
   </si>
   <si>
-    <t>MULTILASER CONNECT</t>
+    <t>CONNECT</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Alpha Desbloqueado Android 4.4 Tela 4.7" 32GB 4G Wi-Fi Camera 12MP - Preto</t>
@@ -2587,7 +2587,7 @@
     <t>Smartphone Blu Studio C Mini D670l, Android 4.4, Dual Chip, Cam 5mp, Mem 4gb, Tela 4.7, 3g - Pret</t>
   </si>
   <si>
-    <t>BLU STUDIO C MINI</t>
+    <t>STUDIO C MINI</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto E Desbloqueado Android 4.4 Tela 4.3" 4GB 3G Wi-Fi Camera 5MP GPS - Preto</t>
@@ -2605,7 +2605,7 @@
     <t>Smartphone Samsung Galaxy Gran Neo Plus Duos Dual Chip Desbloqueado Android 4.4 Tela 5" 8GB 3G Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY GRAN NEO PLUS DUOS</t>
+    <t>GALAXY GRAN NEO PLUS DUOS</t>
   </si>
   <si>
     <t>Smartphone LG G2 lite Dual Chip Desbloqueado Android 4.4 Kit Kat 4.5 Polegadas 4GB 3G Wi-Fi Camera 8MP - Branco</t>
@@ -2614,7 +2614,7 @@
     <t>Smartphone Samsung Galaxy E7 Duos, Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY E7 DUOS</t>
+    <t>GALAXY E7 DUOS</t>
   </si>
   <si>
     <t>Smartphone Motorola Moto G 3a Geracao Colors HDTV Dual Chip Desbloqueado Android 5.1 Tela HD 5" Memoria Interna 16GB 4G Camera 13MP Processador Quad Core 1.4GHz - Branco</t>
@@ -2644,7 +2644,7 @@
     <t>Smartphone Blackberry Bold 9900. Desbloqueado. Tela 2.8". Camera 5.0MP. 3G. Wi Fi e Memoria Interna 768MB</t>
   </si>
   <si>
-    <t>BLACKBERRY BOLD</t>
+    <t>BOLD</t>
   </si>
   <si>
     <t>Smartphone Sony Xperia Z1 Desbloqueado Android 4.2 Tela 5" 16GB 4G Wi-Fi Camera 20MP - Preto</t>
@@ -2674,7 +2674,7 @@
     <t>Smartphone Blu Studio 6.0 Hd, Android 4.2, Dual Chip, Camera 8mp, Mem 4gb, Tela 6.0, 4g - Preto</t>
   </si>
   <si>
-    <t>BLU STUDIO 6.0 HD</t>
+    <t>STUDIO 6.0 HD</t>
   </si>
   <si>
     <t>Smartphone Blu Studio C Mini D670l, Android 4.4, Dual Chip, Cam 5mp, Mem 4gb, Tela 4.7, 3g - Azul</t>
@@ -2689,7 +2689,7 @@
     <t>Smartphone Positivo X400 Dual Chip Desbloqueado Android 4.4 Tela 5" 4GB 3G Wi-Fi Camera 5MP - Preto</t>
   </si>
   <si>
-    <t>POSITIVO X400</t>
+    <t>X400</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy Fame Duos Dual Chip Desbloqueado Android 4.1 Tela 3.5" 3G Wi-Fi Camera 5 MP - Grafite</t>
@@ -2716,7 +2716,7 @@
     <t>Smartphone Samsung Galaxy A7 Dual Chip Desbloqueado Android 4.4 Tela 5.5" 16GB 4G Wi-Fi Camera 13MP - Branco</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY A7</t>
+    <t>GALAXY A7</t>
   </si>
   <si>
     <t>Smartphone Samsung Galaxy A7 Duos Dual Chip Desbloqueado Android 4.4 Tela 5.5" 16GB Wi-Fi 4G Camera 13MP - Dourado</t>
@@ -2743,7 +2743,7 @@
     <t>Smartphone Positivo S480 Dual Chip Desbloqueado Android 4.4 Memoria Interna 8GB 3G Camera 8MP GPS - Preto</t>
   </si>
   <si>
-    <t>POSITIVO S480</t>
+    <t>S480</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 930 Desbloqueado Windows 8.1 32GB 4G Wi-Fi Camera 20MP - Preto</t>
@@ -2752,7 +2752,7 @@
     <t>Smartphone Samsung Galaxy SIII Duos Dual Chip Desbloqueado Claro Android 4.1 Tela 4.3" 8GB 3G Wi-Fi Camera 5MP - Azul</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY SIII DUOS</t>
+    <t>GALAXY SIII DUOS</t>
   </si>
   <si>
     <t>Smartphone Nokia Lumia 530 Desbloqueado Windows Phone 8.1 Tela 4" 4GB 3G Wi-Fi Camera 5MP - Preto + Capa Laranja</t>
@@ -2806,7 +2806,7 @@
     <t>Smartphone Samsung Galaxy E7 Dual Chip Desbloqueado Android 4.4 Tela 5.5" 16GB 4G Wi-Fi Camera 13MP - Preto</t>
   </si>
   <si>
-    <t>SAMSUNG GALAXY E7</t>
+    <t>GALAXY E7</t>
   </si>
   <si>
     <t>Smartphone Galaxy Gran Prime Duos Chip Desbloqueado Oi Android 4.4 Tela 5" 8GB 3G Wi-Fi Camera 8MP - Cinza</t>
@@ -3688,17 +3688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E911"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A911" sqref="A911"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="85.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>